<commit_message>
Issue#25 Req 5.1  abandon Matcher to create Unified Model  implement menteesAssigned at ConverterSAP level
</commit_message>
<xml_diff>
--- a/SAP_duplicate_entires.xlsx
+++ b/SAP_duplicate_entires.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>First name</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Personnel Subarea</t>
+  </si>
+  <si>
+    <t>Kurek</t>
   </si>
 </sst>
 </file>
@@ -927,7 +930,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
@@ -1022,7 +1025,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue#30  Req 5.4  GREEN  add multiple unit tests for leaver status in Mentoring Model  add unit test for seniority conversion
</commit_message>
<xml_diff>
--- a/SAP_duplicate_entires.xlsx
+++ b/SAP_duplicate_entires.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>First name</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Personnel Subarea</t>
-  </si>
-  <si>
-    <t>Kurek</t>
   </si>
 </sst>
 </file>
@@ -930,7 +927,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
@@ -1025,7 +1022,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>